<commit_message>
Modulo envio de correo finalizado
</commit_message>
<xml_diff>
--- a/Data/TEST/Informe VZ ES - copia.xlsx
+++ b/Data/TEST/Informe VZ ES - copia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup-my.sharepoint.com/personal/roboticprocessautomation_rpa1_stihl_es/Documents/Documents/UiPath/Stihl_LCE4_RT1_02_LimitesDeCredito/Data/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup-my.sharepoint.com/personal/roboticprocessautomation_rpa1_stihl_es/Documents/Documents/UiPath/Stihl_LCE4_RT1_02_LimitesDeCredito/Data/TEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="7" documentId="8_{5DC73DCD-B006-4DA5-96E5-8581EDCD0752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDEF6859-146F-45D4-91A2-D6364EF28EE8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D75610A3-A1C5-4597-A58B-667469871DF2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D75610A3-A1C5-4597-A58B-667469871DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="2" r:id="rId1"/>
@@ -31415,14 +31415,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -31433,7 +31433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -31441,7 +31441,7 @@
         <v>19560.190000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -31449,7 +31449,7 @@
         <v>18611.010000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -31457,7 +31457,7 @@
         <v>949.18000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -31465,7 +31465,7 @@
         <v>2055.6999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -31473,7 +31473,7 @@
         <v>2025.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -31481,7 +31481,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
@@ -31489,7 +31489,7 @@
         <v>20109.089999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -31497,7 +31497,7 @@
         <v>196.6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
@@ -31505,7 +31505,7 @@
         <v>19912.489999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
@@ -31513,7 +31513,7 @@
         <v>477.07000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -31521,7 +31521,7 @@
         <v>477.07000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
@@ -31529,7 +31529,7 @@
         <v>2970.68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -31537,7 +31537,7 @@
         <v>2970.68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -31545,7 +31545,7 @@
         <v>4721.7800000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -31553,7 +31553,7 @@
         <v>4676.2700000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
@@ -31561,7 +31561,7 @@
         <v>45.510000000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -31569,7 +31569,7 @@
         <v>439.22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
@@ -31577,7 +31577,7 @@
         <v>439.22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
@@ -31585,7 +31585,7 @@
         <v>24464.18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>13</v>
       </c>
@@ -31593,7 +31593,7 @@
         <v>24133.79</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>21</v>
       </c>
@@ -31601,7 +31601,7 @@
         <v>330.39</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
@@ -31609,7 +31609,7 @@
         <v>16403.21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>15</v>
       </c>
@@ -31617,7 +31617,7 @@
         <v>370.79</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>23</v>
       </c>
@@ -31625,7 +31625,7 @@
         <v>16032.42</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>24</v>
       </c>
@@ -31646,50 +31646,50 @@
   <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.09765625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23.5" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="31.875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.3984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="31.8984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.09765625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.75" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.09765625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.69921875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -31805,7 +31805,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>+VLOOKUP($C2,[1]Zona!$A:$N,14,0)</f>
         <v>Zona 2</v>
@@ -31935,14 +31935,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -32181,21 +32179,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38D7E573-40CC-43AE-A4FF-429148CF4674}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B900B0A-4106-41B5-B5EE-CB317993BA42}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
-    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -32220,9 +32217,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B900B0A-4106-41B5-B5EE-CB317993BA42}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38D7E573-40CC-43AE-A4FF-429148CF4674}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
+    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>